<commit_message>
Ran tests for distributions upload
</commit_message>
<xml_diff>
--- a/public/sample_uploads/capital_distributions.xlsx
+++ b/public/sample_uploads/capital_distributions.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\thimmaiah\work\IRM\public\sample_uploads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A962081-CDC9-4725-A5AE-29527F9E5E20}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB853390-E7C6-4AA0-8E37-8A91D028F597}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="24196" windowHeight="14476" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -413,7 +413,7 @@
   <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView tabSelected="1" showOutlineSymbols="0" showWhiteSpace="0" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.35"/>
@@ -512,7 +512,7 @@
         <v>44866</v>
       </c>
       <c r="F4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G4" t="s">
         <v>11</v>

</xml_diff>

<commit_message>
Added fund docs import call/dist name
</commit_message>
<xml_diff>
--- a/public/sample_uploads/capital_distributions.xlsx
+++ b/public/sample_uploads/capital_distributions.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\thimmaiah\work\IRM\public\sample_uploads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94A890A6-A249-42BC-BB9D-5E870CA74BF9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E289BC7F-B21A-4B62-AC9F-EEF83A1E6444}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="24196" windowHeight="14476" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -61,9 +61,6 @@
     <t>Reinvestment *</t>
   </si>
   <si>
-    <t>Cost Of Investment *</t>
-  </si>
-  <si>
     <t>Type</t>
   </si>
   <si>
@@ -101,6 +98,9 @@
   </si>
   <si>
     <t>INR</t>
+  </si>
+  <si>
+    <t>Face Value For Redemption *</t>
   </si>
 </sst>
 </file>
@@ -455,7 +455,7 @@
   <dimension ref="A1:O4"/>
   <sheetViews>
     <sheetView tabSelected="1" showOutlineSymbols="0" showWhiteSpace="0" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="O4" sqref="O4"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.35"/>
@@ -464,7 +464,7 @@
     <col min="2" max="2" width="13.1875" customWidth="1"/>
     <col min="3" max="3" width="27.5" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="17.625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.625" customWidth="1"/>
+    <col min="5" max="5" width="28.9375" customWidth="1"/>
     <col min="6" max="7" width="14.3125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="16.875" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="12.875" bestFit="1" customWidth="1"/>
@@ -475,7 +475,7 @@
         <v>3</v>
       </c>
       <c r="B1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C1" t="s">
         <v>4</v>
@@ -484,7 +484,7 @@
         <v>5</v>
       </c>
       <c r="E1" t="s">
-        <v>13</v>
+        <v>26</v>
       </c>
       <c r="F1" t="s">
         <v>12</v>
@@ -499,22 +499,22 @@
         <v>8</v>
       </c>
       <c r="J1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="K1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="L1" t="s">
+        <v>20</v>
+      </c>
+      <c r="M1" t="s">
         <v>21</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>22</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>23</v>
-      </c>
-      <c r="O1" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.35">
@@ -522,7 +522,7 @@
         <v>11</v>
       </c>
       <c r="B2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C2" t="s">
         <v>0</v>
@@ -546,13 +546,13 @@
         <v>9</v>
       </c>
       <c r="K2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="L2" t="s">
+        <v>24</v>
+      </c>
+      <c r="M2" t="s">
         <v>25</v>
-      </c>
-      <c r="M2" t="s">
-        <v>26</v>
       </c>
       <c r="N2">
         <v>80</v>
@@ -566,7 +566,7 @@
         <v>11</v>
       </c>
       <c r="B3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C3" t="s">
         <v>1</v>
@@ -590,13 +590,13 @@
         <v>10</v>
       </c>
       <c r="K3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="L3" t="s">
+        <v>24</v>
+      </c>
+      <c r="M3" t="s">
         <v>25</v>
-      </c>
-      <c r="M3" t="s">
-        <v>26</v>
       </c>
       <c r="N3">
         <v>81</v>
@@ -610,7 +610,7 @@
         <v>11</v>
       </c>
       <c r="B4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C4" t="s">
         <v>2</v>
@@ -634,13 +634,13 @@
         <v>10</v>
       </c>
       <c r="J4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="L4" t="s">
+        <v>24</v>
+      </c>
+      <c r="M4" t="s">
         <v>25</v>
-      </c>
-      <c r="M4" t="s">
-        <v>26</v>
       </c>
       <c r="N4">
         <v>81</v>

</xml_diff>

<commit_message>
Check for blank exchange rates for import distributions
</commit_message>
<xml_diff>
--- a/public/sample_uploads/capital_distributions.xlsx
+++ b/public/sample_uploads/capital_distributions.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\thimmaiah\work\IRM\public\sample_uploads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E289BC7F-B21A-4B62-AC9F-EEF83A1E6444}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{070AB1E8-BCD0-41CC-A8B1-5BCED6BF8C9B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="24196" windowHeight="14476" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="27">
   <si>
     <t>Distribution from Sale : Aug</t>
   </si>
@@ -455,7 +455,7 @@
   <dimension ref="A1:O4"/>
   <sheetViews>
     <sheetView tabSelected="1" showOutlineSymbols="0" showWhiteSpace="0" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="O4" sqref="O4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.35"/>
@@ -636,18 +636,7 @@
       <c r="J4" t="s">
         <v>17</v>
       </c>
-      <c r="L4" t="s">
-        <v>24</v>
-      </c>
-      <c r="M4" t="s">
-        <v>25</v>
-      </c>
-      <c r="N4">
-        <v>81</v>
-      </c>
-      <c r="O4" s="1">
-        <v>44866</v>
-      </c>
+      <c r="O4" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Import fund units2 (#136)
* Removed unwanted request access btn

* Fixed issue with col=all, renamed to grid specific

* Fixed tests for fund unit imports

* Tests pass for fund unit import
</commit_message>
<xml_diff>
--- a/public/sample_uploads/capital_distributions.xlsx
+++ b/public/sample_uploads/capital_distributions.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\thimmaiah\work\IRM\public\sample_uploads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{070AB1E8-BCD0-41CC-A8B1-5BCED6BF8C9B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD6586B3-6EF8-463F-A6F3-2394C1980E35}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="24196" windowHeight="14476" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,16 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="27">
-  <si>
-    <t>Distribution from Sale : Aug</t>
-  </si>
-  <si>
-    <t>Distribution from Sale : Sept</t>
-  </si>
-  <si>
-    <t>Distribution from Sale : Nov</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="20">
   <si>
     <t>Fund *</t>
   </si>
@@ -52,9 +43,6 @@
     <t>Yes</t>
   </si>
   <si>
-    <t>No</t>
-  </si>
-  <si>
     <t>SAAS Fund</t>
   </si>
   <si>
@@ -67,21 +55,12 @@
     <t>Pool</t>
   </si>
   <si>
-    <t>CoInvest</t>
-  </si>
-  <si>
     <t>Folio No</t>
   </si>
   <si>
-    <t>C1</t>
-  </si>
-  <si>
     <t>Distribution Basis</t>
   </si>
   <si>
-    <t>Commitment Percentage</t>
-  </si>
-  <si>
     <t>From Currency</t>
   </si>
   <si>
@@ -94,13 +73,13 @@
     <t>As Of</t>
   </si>
   <si>
-    <t>USD</t>
-  </si>
-  <si>
-    <t>INR</t>
-  </si>
-  <si>
     <t>Face Value For Redemption *</t>
+  </si>
+  <si>
+    <t>Distribution 1</t>
+  </si>
+  <si>
+    <t>Distribution 2</t>
   </si>
 </sst>
 </file>
@@ -452,10 +431,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:O4"/>
+  <dimension ref="A1:O3"/>
   <sheetViews>
-    <sheetView tabSelected="1" showOutlineSymbols="0" showWhiteSpace="0" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="O4" sqref="O4"/>
+    <sheetView tabSelected="1" showOutlineSymbols="0" showWhiteSpace="0" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.35"/>
@@ -472,60 +451,60 @@
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G1" t="s">
         <v>3</v>
       </c>
-      <c r="B1" t="s">
+      <c r="H1" t="s">
+        <v>4</v>
+      </c>
+      <c r="I1" t="s">
+        <v>5</v>
+      </c>
+      <c r="J1" t="s">
+        <v>11</v>
+      </c>
+      <c r="K1" t="s">
+        <v>12</v>
+      </c>
+      <c r="L1" t="s">
         <v>13</v>
       </c>
-      <c r="C1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D1" t="s">
-        <v>5</v>
-      </c>
-      <c r="E1" t="s">
-        <v>26</v>
-      </c>
-      <c r="F1" t="s">
-        <v>12</v>
-      </c>
-      <c r="G1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" t="s">
-        <v>8</v>
-      </c>
-      <c r="J1" t="s">
+      <c r="M1" t="s">
+        <v>14</v>
+      </c>
+      <c r="N1" t="s">
+        <v>15</v>
+      </c>
+      <c r="O1" t="s">
         <v>16</v>
-      </c>
-      <c r="K1" t="s">
-        <v>18</v>
-      </c>
-      <c r="L1" t="s">
-        <v>20</v>
-      </c>
-      <c r="M1" t="s">
-        <v>21</v>
-      </c>
-      <c r="N1" t="s">
-        <v>22</v>
-      </c>
-      <c r="O1" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="B2" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="C2" t="s">
-        <v>0</v>
+        <v>18</v>
       </c>
       <c r="D2" s="2">
         <v>1000000</v>
@@ -540,36 +519,22 @@
         <v>44743</v>
       </c>
       <c r="H2" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="I2" t="s">
-        <v>9</v>
-      </c>
-      <c r="K2" t="s">
-        <v>19</v>
-      </c>
-      <c r="L2" t="s">
-        <v>24</v>
-      </c>
-      <c r="M2" t="s">
-        <v>25</v>
-      </c>
-      <c r="N2">
-        <v>80</v>
-      </c>
-      <c r="O2" s="1">
-        <v>44743</v>
-      </c>
+        <v>6</v>
+      </c>
+      <c r="O2" s="1"/>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="B3" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="C3" t="s">
-        <v>1</v>
+        <v>19</v>
       </c>
       <c r="D3" s="2">
         <v>2000000</v>
@@ -584,59 +549,12 @@
         <v>44774</v>
       </c>
       <c r="H3" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="I3" t="s">
-        <v>10</v>
-      </c>
-      <c r="K3" t="s">
-        <v>19</v>
-      </c>
-      <c r="L3" t="s">
-        <v>24</v>
-      </c>
-      <c r="M3" t="s">
-        <v>25</v>
-      </c>
-      <c r="N3">
-        <v>81</v>
-      </c>
-      <c r="O3" s="1">
-        <v>44774</v>
-      </c>
-    </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
-        <v>11</v>
-      </c>
-      <c r="B4" t="s">
-        <v>15</v>
-      </c>
-      <c r="C4" t="s">
-        <v>2</v>
-      </c>
-      <c r="D4" s="2">
-        <v>3000000</v>
-      </c>
-      <c r="E4" s="2">
-        <v>2500000</v>
-      </c>
-      <c r="F4" s="2">
-        <v>300000</v>
-      </c>
-      <c r="G4" s="1">
-        <v>44866</v>
-      </c>
-      <c r="H4" t="s">
-        <v>9</v>
-      </c>
-      <c r="I4" t="s">
-        <v>10</v>
-      </c>
-      <c r="J4" t="s">
-        <v>17</v>
-      </c>
-      <c r="O4" s="1"/>
+        <v>6</v>
+      </c>
+      <c r="O3" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Capital Dist fixes (#768)
* Added check for distribution to allow upload CDPs

* Added send_notification_on_complete to CD

* Added send notification col to import CD

* Added completed_distribution_amount_cents to CD

* Fixed tests
</commit_message>
<xml_diff>
--- a/public/sample_uploads/capital_distributions.xlsx
+++ b/public/sample_uploads/capital_distributions.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\thimmaiah\work\IRM\public\sample_uploads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10CC15B6-15E5-461E-8FF6-8C88E644805D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD52929F-24E3-48E4-BABA-07F7514ECC3D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="24196" windowHeight="14476" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -206,7 +206,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H1" authorId="0" shapeId="0" xr:uid="{C1113430-FE0E-4DBA-8DBA-78F34B985766}">
+    <comment ref="I1" authorId="0" shapeId="0" xr:uid="{C1113430-FE0E-4DBA-8DBA-78F34B985766}">
       <text>
         <r>
           <rPr>
@@ -230,7 +230,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I1" authorId="0" shapeId="0" xr:uid="{58EFFF56-2CD1-427F-A405-11B16D828151}">
+    <comment ref="J1" authorId="0" shapeId="0" xr:uid="{58EFFF56-2CD1-427F-A405-11B16D828151}">
       <text>
         <r>
           <rPr>
@@ -254,7 +254,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J1" authorId="0" shapeId="0" xr:uid="{A0E463FE-5C5B-4B9D-8D9C-E2BE743808EF}">
+    <comment ref="K1" authorId="0" shapeId="0" xr:uid="{A0E463FE-5C5B-4B9D-8D9C-E2BE743808EF}">
       <text>
         <r>
           <rPr>
@@ -278,7 +278,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="K1" authorId="0" shapeId="0" xr:uid="{7B023418-75A9-4D10-8903-532DD8C6B918}">
+    <comment ref="L1" authorId="0" shapeId="0" xr:uid="{7B023418-75A9-4D10-8903-532DD8C6B918}">
       <text>
         <r>
           <rPr>
@@ -303,7 +303,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="L1" authorId="0" shapeId="0" xr:uid="{2ABF67B8-58B2-4AC8-8C17-DAFD69A2DE15}">
+    <comment ref="M1" authorId="0" shapeId="0" xr:uid="{2ABF67B8-58B2-4AC8-8C17-DAFD69A2DE15}">
       <text>
         <r>
           <rPr>
@@ -328,7 +328,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="M1" authorId="0" shapeId="0" xr:uid="{3E9CBC99-5D51-4417-9EF1-14208A629E5E}">
+    <comment ref="N1" authorId="0" shapeId="0" xr:uid="{3E9CBC99-5D51-4417-9EF1-14208A629E5E}">
       <text>
         <r>
           <rPr>
@@ -353,7 +353,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="N1" authorId="0" shapeId="0" xr:uid="{7A6E468D-0F53-4407-92A9-4C75835F66C7}">
+    <comment ref="O1" authorId="0" shapeId="0" xr:uid="{7A6E468D-0F53-4407-92A9-4C75835F66C7}">
       <text>
         <r>
           <rPr>
@@ -383,7 +383,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="19">
   <si>
     <t>Fund *</t>
   </si>
@@ -437,6 +437,9 @@
   </si>
   <si>
     <t>Income *</t>
+  </si>
+  <si>
+    <t>Send Notification</t>
   </si>
 </sst>
 </file>
@@ -842,10 +845,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:N191"/>
+  <dimension ref="A1:O191"/>
   <sheetViews>
     <sheetView tabSelected="1" showOutlineSymbols="0" showWhiteSpace="0" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:B1048576"/>
+      <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.35"/>
@@ -857,17 +860,18 @@
     <col min="5" max="5" width="13.25" style="2" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="9.9375" style="2" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="16.8125" style="2" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13" style="2" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="7.6875" style="2" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="15.5625" style="2" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="13.25" style="2" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="10.9375" style="2" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="13.5" style="2" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="5.1875" style="2" bestFit="1" customWidth="1"/>
-    <col min="15" max="16384" width="9" style="2"/>
+    <col min="8" max="8" width="16.8125" style="2" customWidth="1"/>
+    <col min="9" max="9" width="13" style="2" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="7.6875" style="2" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="15.5625" style="2" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="13.25" style="2" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="10.9375" style="2" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="13.5" style="2" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="5.1875" style="2" bestFit="1" customWidth="1"/>
+    <col min="16" max="16384" width="9" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="13.5" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -890,28 +894,31 @@
         <v>3</v>
       </c>
       <c r="H1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="I1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>6</v>
       </c>
@@ -936,9 +943,12 @@
       <c r="H2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="N2" s="4"/>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="I2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="O2" s="4"/>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
         <v>6</v>
       </c>
@@ -963,45 +973,48 @@
       <c r="H3" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="N3" s="4"/>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="I3" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="O3" s="4"/>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.35">
       <c r="D4" s="3"/>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.35">
       <c r="D5" s="3"/>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.35">
       <c r="D6" s="3"/>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.35">
       <c r="D7" s="3"/>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.35">
       <c r="D8" s="3"/>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.35">
       <c r="D9" s="3"/>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.35">
       <c r="D10" s="3"/>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.35">
       <c r="D11" s="3"/>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.35">
       <c r="D12" s="3"/>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.35">
       <c r="D13" s="3"/>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.35">
       <c r="D14" s="3"/>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.35">
       <c r="D15" s="3"/>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.35">
       <c r="D16" s="3"/>
     </row>
     <row r="17" spans="4:4" x14ac:dyDescent="0.35">
@@ -1532,7 +1545,7 @@
   </sheetData>
   <dataValidations count="2">
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Amount cannot be more than the Gross amount" prompt="Less than / equal to gross amout" sqref="D2:D191" xr:uid="{73646F8A-D872-4509-8942-D1241A841B31}"/>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:H191" xr:uid="{B8321C99-7069-4443-A0C1-F2F3B192133C}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:I191" xr:uid="{B8321C99-7069-4443-A0C1-F2F3B192133C}">
       <formula1>"Yes,No"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>